<commit_message>
mod: rename IO_GENERATOR to LOGIC_GENERATOR
</commit_message>
<xml_diff>
--- a/EXCEL_MASTER.xlsx
+++ b/EXCEL_MASTER.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\2025\ScriptGenerator\Code\toDeploy\V2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\2025\ScriptGenerator\Code\toDeploy\logic_designer_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F99C4CE-5647-4272-87C3-74ECB1106CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC7C9A3B-8539-4580-A7BE-C270938BEA0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{CA16010F-BA2C-49E5-B591-C71559C6A31C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CA16010F-BA2C-49E5-B591-C71559C6A31C}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="9" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="248">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -122,12 +122,6 @@
     <t>PID</t>
   </si>
   <si>
-    <t>SIO22</t>
-  </si>
-  <si>
-    <t>SIO12</t>
-  </si>
-  <si>
     <t>SIO21</t>
   </si>
   <si>
@@ -167,21 +161,12 @@
     <t>Please enter your IO data into EVERY column on the relevant TYPE of the type sheet*</t>
   </si>
   <si>
-    <t>Put the ExcelMaster_IOGenerator.xlsx file on the same folder as the IOGenerator.exe file</t>
-  </si>
-  <si>
-    <t>Execute the IOGenerator.exe</t>
-  </si>
-  <si>
     <t>Filling up the excel file:</t>
   </si>
   <si>
     <t>Guide to Use The IOGenerator Engineering Tools</t>
   </si>
   <si>
-    <t>Using the output file:</t>
-  </si>
-  <si>
     <t>Sheet</t>
   </si>
   <si>
@@ -194,165 +179,12 @@
     <t>Fill the first column with "TYPE" (without " ") on every row that has IO Data</t>
   </si>
   <si>
-    <t>LALL_9056A</t>
-  </si>
-  <si>
-    <t>Level Lo Lo</t>
-  </si>
-  <si>
-    <t>LAHH_9056A</t>
-  </si>
-  <si>
-    <t>Level Hi Hi</t>
-  </si>
-  <si>
-    <t>FD_001</t>
-  </si>
-  <si>
-    <t>FireDetector</t>
-  </si>
-  <si>
     <t>I_Anlg</t>
   </si>
   <si>
     <t>%</t>
   </si>
   <si>
-    <t>CV_001</t>
-  </si>
-  <si>
-    <t>Control Valve 001</t>
-  </si>
-  <si>
-    <t>LT_004</t>
-  </si>
-  <si>
-    <t>Level Transmitter</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>P_5505</t>
-  </si>
-  <si>
-    <t>Pump Hz</t>
-  </si>
-  <si>
-    <t>Hz</t>
-  </si>
-  <si>
-    <t>ZSO_555</t>
-  </si>
-  <si>
-    <t>Valve 555 Open Status</t>
-  </si>
-  <si>
-    <t>ZSC_555</t>
-  </si>
-  <si>
-    <t>Valve 555 Close Status</t>
-  </si>
-  <si>
-    <t>XVO_555</t>
-  </si>
-  <si>
-    <t>Valve 555 Command Open</t>
-  </si>
-  <si>
-    <t>XVC_555</t>
-  </si>
-  <si>
-    <t>Valve 555 Command Close</t>
-  </si>
-  <si>
-    <t>XV_555</t>
-  </si>
-  <si>
-    <t>Valve 555</t>
-  </si>
-  <si>
-    <t>ZS_551</t>
-  </si>
-  <si>
-    <t>Valve 551 o/c status</t>
-  </si>
-  <si>
-    <t>XVO_551</t>
-  </si>
-  <si>
-    <t>Valve 551 command open</t>
-  </si>
-  <si>
-    <t>XVC_551</t>
-  </si>
-  <si>
-    <t>Valve 551 command close</t>
-  </si>
-  <si>
-    <t>XV_551</t>
-  </si>
-  <si>
-    <t>Valve 551</t>
-  </si>
-  <si>
-    <t>ZSO_552</t>
-  </si>
-  <si>
-    <t>ZSC_552</t>
-  </si>
-  <si>
-    <t>Valve 552 Open Status</t>
-  </si>
-  <si>
-    <t>Valve 552 Close Status</t>
-  </si>
-  <si>
-    <t>XVC_552</t>
-  </si>
-  <si>
-    <t>Valve 552 Command</t>
-  </si>
-  <si>
-    <t>XV_552</t>
-  </si>
-  <si>
-    <t>Valve 552</t>
-  </si>
-  <si>
-    <t>Valve 554 Open Status</t>
-  </si>
-  <si>
-    <t>Valve 554 Command Open</t>
-  </si>
-  <si>
-    <t>XVC_554</t>
-  </si>
-  <si>
-    <t>XV_554</t>
-  </si>
-  <si>
-    <t>Valve 554</t>
-  </si>
-  <si>
-    <t>ZS_554</t>
-  </si>
-  <si>
-    <t>LT_552</t>
-  </si>
-  <si>
-    <t>Level Tank 552</t>
-  </si>
-  <si>
-    <t>LCV_552</t>
-  </si>
-  <si>
-    <t>Level Control Valve Tank 552</t>
-  </si>
-  <si>
-    <t>Level Control Valve PID</t>
-  </si>
-  <si>
     <t>TAG_IN1</t>
   </si>
   <si>
@@ -365,20 +197,608 @@
     <t>TAG_OUT2</t>
   </si>
   <si>
-    <t>SIO11</t>
-  </si>
-  <si>
     <t>For analog input, please specify ANLG_IN_TYPE (I_Anlg or I_Temp)</t>
   </si>
   <si>
-    <t>I_Temp</t>
+    <t>ESD-000</t>
+  </si>
+  <si>
+    <t>DP-UPS-01B</t>
+  </si>
+  <si>
+    <t>ESD-001</t>
+  </si>
+  <si>
+    <t>ESD-002</t>
+  </si>
+  <si>
+    <t>MCC-ON</t>
+  </si>
+  <si>
+    <t>MCC-TRIP</t>
+  </si>
+  <si>
+    <t>MCC-ALRM</t>
+  </si>
+  <si>
+    <t>PSD-81001</t>
+  </si>
+  <si>
+    <t>PSD-82001</t>
+  </si>
+  <si>
+    <t>PSD-83001</t>
+  </si>
+  <si>
+    <t>PSD-84001</t>
+  </si>
+  <si>
+    <t>PSD-85001</t>
+  </si>
+  <si>
+    <t>PSD-86001</t>
+  </si>
+  <si>
+    <t>ESD-PB</t>
+  </si>
+  <si>
+    <t>PSD-000</t>
+  </si>
+  <si>
+    <t>PSD-PB</t>
+  </si>
+  <si>
+    <t>UPS Indicator</t>
+  </si>
+  <si>
+    <t>ESD-PB 1 - Gas Compressor Area - North of Overhaul Area</t>
+  </si>
+  <si>
+    <t>ESD-PB 2 - Filter Area - South Fence Near Hydrant</t>
+  </si>
+  <si>
+    <t>MCC GBC (New Elec Room) Status ON</t>
+  </si>
+  <si>
+    <t>MCC GBC (New Elec Room) Status TRIP</t>
+  </si>
+  <si>
+    <t>MCC GBC (New Elec Room) Status ALARM</t>
+  </si>
+  <si>
+    <t>Process Shutdown from K-8100</t>
+  </si>
+  <si>
+    <t>Process Shutdown from K-8200</t>
+  </si>
+  <si>
+    <t>Process Shutdown from K-8300</t>
+  </si>
+  <si>
+    <t>Process Shutdown from K-8400</t>
+  </si>
+  <si>
+    <t>Process Shutdown from K-8500</t>
+  </si>
+  <si>
+    <t>Process Shutdown from K-8600</t>
+  </si>
+  <si>
+    <t>ESD Push Button from ESS Panel</t>
+  </si>
+  <si>
+    <t>PSD Push Button from ESS Existing Panel Train #2</t>
+  </si>
+  <si>
+    <t>PSD Push Button from ESS Panel</t>
+  </si>
+  <si>
+    <t>ESD Push Button from ESS Existing Panel Train #2</t>
+  </si>
+  <si>
+    <t>ESD-8810</t>
+  </si>
+  <si>
+    <t>ESD-8820</t>
+  </si>
+  <si>
+    <t>ESD-IND</t>
+  </si>
+  <si>
+    <t>XL-001A</t>
+  </si>
+  <si>
+    <t>XA-001</t>
+  </si>
+  <si>
+    <t>XL-001B</t>
+  </si>
+  <si>
+    <t>XL-002A</t>
+  </si>
+  <si>
+    <t>XA-002</t>
+  </si>
+  <si>
+    <t>XL-002B</t>
+  </si>
+  <si>
+    <t>MCC-ESD-01</t>
+  </si>
+  <si>
+    <t>MCC-ESD-02</t>
+  </si>
+  <si>
+    <t>MCC-ESD-03</t>
+  </si>
+  <si>
+    <t>MCC-ESD-04</t>
+  </si>
+  <si>
+    <t>MCC-ESD-05</t>
+  </si>
+  <si>
+    <t>MCC-ESD-06</t>
+  </si>
+  <si>
+    <t>MCC-ESD-07</t>
+  </si>
+  <si>
+    <t>MCC-ESD-08</t>
+  </si>
+  <si>
+    <t>MCC-ESD-09</t>
+  </si>
+  <si>
+    <t>GAS-COMP-TRIP</t>
+  </si>
+  <si>
+    <t>P-5030-STA</t>
+  </si>
+  <si>
+    <t>ESD Command K-8810</t>
+  </si>
+  <si>
+    <t>ESD Command K-8820</t>
+  </si>
+  <si>
+    <t>ESD Indication To Existing ESS Control Panel</t>
+  </si>
+  <si>
+    <t>Strobe Light 1A - Office Area</t>
+  </si>
+  <si>
+    <t>Horn 1 - Office Area</t>
+  </si>
+  <si>
+    <t>Strobe Light 1B - Office Area</t>
+  </si>
+  <si>
+    <t>Strobe Light 2A - Field Area</t>
+  </si>
+  <si>
+    <t>Horn 2 - Field Area</t>
+  </si>
+  <si>
+    <t>Strobe Light 2B - Field Area</t>
+  </si>
+  <si>
+    <t>Utility - MCC Trip Command</t>
+  </si>
+  <si>
+    <t>DP-UPS - MCC Trip Command 1/2</t>
+  </si>
+  <si>
+    <t>DP-UPS - MCC Trip Command 2/2</t>
+  </si>
+  <si>
+    <t>Crane Shelter Gas Comp - MCC Trip Command</t>
+  </si>
+  <si>
+    <t>i/A -  MCC Trip Command 1/2</t>
+  </si>
+  <si>
+    <t>i/A -  MCC Trip Command 2/2</t>
+  </si>
+  <si>
+    <t>Demin Water - MCC Trip Command</t>
+  </si>
+  <si>
+    <t>Waste Trf Pump - MCC Trip Command</t>
+  </si>
+  <si>
+    <t>N2 Gen - MCC Trip Command</t>
+  </si>
+  <si>
+    <t>Gas Compressor Signal Trip to Aux Panel in Existing Control Room</t>
+  </si>
+  <si>
+    <t>P-5030 Start Signal to Aux Panel Train # 2</t>
+  </si>
+  <si>
+    <t>PZT-80101</t>
+  </si>
+  <si>
+    <t>LZT-80102</t>
+  </si>
+  <si>
+    <t>LZT-80302</t>
+  </si>
+  <si>
+    <t>PZT-80403</t>
+  </si>
+  <si>
+    <t>PT-80702</t>
+  </si>
+  <si>
+    <t>PT-80901</t>
+  </si>
+  <si>
+    <t>PT - Separator V-8010</t>
+  </si>
+  <si>
+    <t>LT - Separator V-8010</t>
+  </si>
+  <si>
+    <t>LT - Discharge Gas Scrubber V-8030</t>
+  </si>
+  <si>
+    <t>PT - Out Gas to Exist Amine Plant Line P-8042-DS-10"</t>
+  </si>
+  <si>
+    <t>PT - Inlet of FG Filter Coalescer</t>
+  </si>
+  <si>
+    <t>PT - Instrument Air Receiver V-8090</t>
+  </si>
+  <si>
+    <t>GD-001</t>
+  </si>
+  <si>
+    <t>GD-002</t>
+  </si>
+  <si>
+    <t>GD-003</t>
+  </si>
+  <si>
+    <t>GD-004</t>
+  </si>
+  <si>
+    <t>GD-005</t>
+  </si>
+  <si>
+    <t>GD-006</t>
+  </si>
+  <si>
+    <t>GD-007</t>
+  </si>
+  <si>
+    <t>GD-008</t>
+  </si>
+  <si>
+    <t>GD-009</t>
+  </si>
+  <si>
+    <t>GD-001-H2S</t>
+  </si>
+  <si>
+    <t>GD-002-H2S</t>
+  </si>
+  <si>
+    <t>GD-003-H2S</t>
+  </si>
+  <si>
+    <t>GD-004-H2S</t>
+  </si>
+  <si>
+    <t>GD-005-H2S</t>
+  </si>
+  <si>
+    <t>Gas Detector 1 - K-8100</t>
+  </si>
+  <si>
+    <t>Gas Detector 2 - K-8200</t>
+  </si>
+  <si>
+    <t>Gas Detector 3- K-8300</t>
+  </si>
+  <si>
+    <t>Gas Detector 4 - K-8400</t>
+  </si>
+  <si>
+    <t>Gas Detector 5 - K-8500</t>
+  </si>
+  <si>
+    <t>Gas Detector 6 - K-8600</t>
+  </si>
+  <si>
+    <t>Gas Detector 7 - Fuel Gas Filter Area F-8070A/B</t>
+  </si>
+  <si>
+    <t>Gas Detector 8 - Discharge Gas Filter F-8040A/B</t>
+  </si>
+  <si>
+    <t>Gas Detector 9 - Suction Gas Filter F-8020A/B</t>
+  </si>
+  <si>
+    <t>H2S Gas Detector 1 - K-8100</t>
+  </si>
+  <si>
+    <t>H2S Gas Detector 2 - K-8200</t>
+  </si>
+  <si>
+    <t>H2S Gas Detector 3 - K-8300</t>
+  </si>
+  <si>
+    <t>H2S Gas Detector 4 - K-8400</t>
+  </si>
+  <si>
+    <t>H2S Gas Detector 5 - K-8500</t>
+  </si>
+  <si>
+    <t>GD-006-H2S</t>
+  </si>
+  <si>
+    <t>GD-007-H2S</t>
+  </si>
+  <si>
+    <t>GD-008-H2S</t>
+  </si>
+  <si>
+    <t>GD-009-H2S</t>
+  </si>
+  <si>
+    <t>FD-001</t>
+  </si>
+  <si>
+    <t>FD-002</t>
+  </si>
+  <si>
+    <t>FD-003</t>
+  </si>
+  <si>
+    <t>FD-004</t>
+  </si>
+  <si>
+    <t>FD-005</t>
+  </si>
+  <si>
+    <t>FD-006</t>
+  </si>
+  <si>
+    <t>FD-007</t>
+  </si>
+  <si>
+    <t>FD-008</t>
+  </si>
+  <si>
+    <t>FD-009</t>
+  </si>
+  <si>
+    <t>FD-010</t>
+  </si>
+  <si>
+    <t>H2S Gas Detector 6 - K-8600</t>
+  </si>
+  <si>
+    <t>H2S Gas Detector 7 - Fuel Gas Filter Area F-8070A/B</t>
+  </si>
+  <si>
+    <t>H2S Gas Detector 8 - Discharge Gas Filter F-8040A/B</t>
+  </si>
+  <si>
+    <t>H2S Gas Detector 9 - Suction Gas Filter F-8020A/B</t>
+  </si>
+  <si>
+    <t>Flame Detector 1 - North Fence K-8100/8200</t>
+  </si>
+  <si>
+    <t>Flame Detector 2 - South Fence K-8100/8200</t>
+  </si>
+  <si>
+    <t>Flame Detector 3 - North Fence K-8300/8400</t>
+  </si>
+  <si>
+    <t>Flame Detector 4 - South Fence K-8300/8400</t>
+  </si>
+  <si>
+    <t>Flame Detector 5 - North Fence K-8500/8600</t>
+  </si>
+  <si>
+    <t>Flame Detector 6 - South Fence K-8500/8600</t>
+  </si>
+  <si>
+    <t>Flame Detector 7 - West Fence Filter Area</t>
+  </si>
+  <si>
+    <t>Flame Detector 8 - South Fence Filter Area</t>
+  </si>
+  <si>
+    <t>Flame Detector 9 - East Fence Filter Area</t>
+  </si>
+  <si>
+    <t>Flame Detector 10 - North Fence Filter Area</t>
+  </si>
+  <si>
+    <t>ZSC-80101</t>
+  </si>
+  <si>
+    <t>ZSO-80101</t>
+  </si>
+  <si>
+    <t>Valve Close Status - Inlet of Separator SDV-80101</t>
+  </si>
+  <si>
+    <t>Valve Open Status - Inlet of Separator SDV-80101</t>
+  </si>
+  <si>
+    <t>SDY-80101</t>
+  </si>
+  <si>
+    <t>3-Way SV - Inlet of Separator SDV-80101</t>
+  </si>
+  <si>
+    <t>SDV_80101</t>
+  </si>
+  <si>
+    <t>ZSC-80102</t>
+  </si>
+  <si>
+    <t>ZSO-80102</t>
+  </si>
+  <si>
+    <t>Valve Close Status - Gas Outlet of Separator BDV-80102</t>
+  </si>
+  <si>
+    <t>Valve Open Status - Gas Outlet of Separator BDV-80102</t>
+  </si>
+  <si>
+    <t>BDY-80102</t>
+  </si>
+  <si>
+    <t>3-Way SV - Gas Outlet of Separator BDV-80102</t>
+  </si>
+  <si>
+    <t>BDV_80102</t>
+  </si>
+  <si>
+    <t>ZSC-80103</t>
+  </si>
+  <si>
+    <t>ZSO-80103</t>
+  </si>
+  <si>
+    <t>Valve Open Status - Line to HC Liquid Header SDV-80103</t>
+  </si>
+  <si>
+    <t>Valve Close Status - Line to HC Liquid Header SDV-80103</t>
+  </si>
+  <si>
+    <t>SDY-80103</t>
+  </si>
+  <si>
+    <t>3-Way SV - Line to HC Liquid Header SDV-80103</t>
+  </si>
+  <si>
+    <t>SDV_80103</t>
+  </si>
+  <si>
+    <t>Note.</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>DON'T REMOVE ANY SHEET OR MODIFY THE ORDER OF THE SHEETS. ONLY MODIFY CELLS/CONTENT OF THE SHEET</t>
+  </si>
+  <si>
+    <t>All of the output files will be generate at {.exe directory}/Output folder</t>
+  </si>
+  <si>
+    <t>Those files are:</t>
+  </si>
+  <si>
+    <t>STRUCT_TEXT.txt</t>
+  </si>
+  <si>
+    <t>LOC_VAR.xlsx</t>
+  </si>
+  <si>
+    <t>DEV_LABEL.csv</t>
+  </si>
+  <si>
+    <t>MASTER.csv is also generated at {.exe directory} and is read by the LogicGenerator.exe in lines (not to be used for LogicDesigner)</t>
+  </si>
+  <si>
+    <t>Output Files:</t>
+  </si>
+  <si>
+    <t>Open Logic Designer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">. </t>
+  </si>
+  <si>
+    <t>Open Device Label Definition, and choose 'READING. . .'</t>
+  </si>
+  <si>
+    <t>Select DEV_LABEL.csv in the Output folder. Import option can be filled accordingly.</t>
+  </si>
+  <si>
+    <t>Put the EXCEL_MASTER.xlsx file on the same folder as the LOGIC_GENERATOR.exe file</t>
+  </si>
+  <si>
+    <t>Execute the LOGIC_GENERATOR.exe</t>
+  </si>
+  <si>
+    <t>Importing DEV_LABEL.csv to DeviceLabelDefinition</t>
+  </si>
+  <si>
+    <t>After creating a new project, insert a program</t>
+  </si>
+  <si>
+    <t>Select ST as the language</t>
+  </si>
+  <si>
+    <t>Copy all text inside the STRUCT_TEXT.txt file and paste it to the worksheet of the program</t>
+  </si>
+  <si>
+    <t>Copying the Local Variables from LOC_VAR.xlsx</t>
+  </si>
+  <si>
+    <t>After pasting the script into the worksheet, copy all the variables generated into the POU.</t>
+  </si>
+  <si>
+    <t>Rearrange the header of the variable table of the POU into --&gt; Name, Type, Desc, Usage, Retain</t>
+  </si>
+  <si>
+    <t>Add/append/insert a new variable</t>
+  </si>
+  <si>
+    <t>Copy all the variables from LOC_VAR.xlsx</t>
+  </si>
+  <si>
+    <t>Add the POU into Task</t>
+  </si>
+  <si>
+    <t>Copying the Script from STRUCT_TEXT.txt into a new POU</t>
+  </si>
+  <si>
+    <t>Paste into the NewVar1. When asked this dialogue, select 'Yes'</t>
+  </si>
+  <si>
+    <t>Continue adding the device label into the project</t>
+  </si>
+  <si>
+    <t>Rebuild the project. By default, there should be 0 error and 0 warning after the rebuild.</t>
+  </si>
+  <si>
+    <t>If face with an error, please recheck your EXCEL_MASTER.xlsx for wrong data input</t>
+  </si>
+  <si>
+    <t>Using 'Source Conversion' Tool in Logic Designer</t>
+  </si>
+  <si>
+    <t>After a successful rebuild, right click on the POU and run Logic Designer Conversion Tool to convert ST into FBD language</t>
+  </si>
+  <si>
+    <t>Select 'Convert to: FBD' in the radio button. If you select 'Overwrite source POU', the converter will overwrite the script POU</t>
+  </si>
+  <si>
+    <t>The converted POU will have several worksheet and each type of NPAS will be separated by comment</t>
+  </si>
+  <si>
+    <t>Add the new POU into the Task. Do rearrange as needed since the conversion file is untidy</t>
+  </si>
+  <si>
+    <t>The pre-filled value is set as an example</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -398,6 +818,20 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -423,7 +857,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -431,11 +865,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -453,11 +902,92 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -468,6 +998,582 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>65942</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>21982</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>2080846</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3B6CE7E-525D-4AC5-9DBF-8885DC376268}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect r="1546" b="9562"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="608134" y="6205905"/>
+          <a:ext cx="2476501" cy="2058864"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>157528</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>2036885</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C433754E-BD4B-F9F0-2A7B-0D4470AE6A5B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="608135" y="8499232"/>
+          <a:ext cx="3564547" cy="2036884"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>168520</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>4030491</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB29899A-6127-29D9-395A-D85586E765B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="608136" y="10763251"/>
+          <a:ext cx="3575538" cy="4030490"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>300766</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>1370135</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC795366-5025-2A34-7E4F-DA22A10E17DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="608135" y="15401192"/>
+          <a:ext cx="3099650" cy="1370135"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>58616</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>2638693</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A160221-5E91-F32F-2337-4E71E6B6132E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="542192" y="16983809"/>
+          <a:ext cx="2923443" cy="2638692"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>481476</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>2535116</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07212F57-9FE8-B6E4-9594-337471BD2E88}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="608136" y="19870616"/>
+          <a:ext cx="4496628" cy="2535115"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>26748</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>1970943</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95919998-7F84-81E9-4F4C-D220AF88E018}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="608136" y="23109115"/>
+          <a:ext cx="5258170" cy="1970943"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>1247602</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8E3F42E-3066-67D3-D5C7-CB3868F62609}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="608135" y="25307192"/>
+          <a:ext cx="5231423" cy="1247602"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>234461</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>2066701</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47D7C8FC-493E-F6C5-F707-74172EA793AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="608135" y="26838519"/>
+          <a:ext cx="2425211" cy="2066701"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>403513</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>1638529</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39DC56B4-9899-7A50-0E10-CDF7056FAEB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="608135" y="29490865"/>
+          <a:ext cx="3810532" cy="1638529"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>600808</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>2111514</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77FB7D85-C8D7-9F70-69EE-E7AF0EAB9FB8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="608135" y="32319058"/>
+          <a:ext cx="2183423" cy="2111514"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>315057</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>1844553</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC1254FB-E8DD-58B0-DDCB-8BF1A772E901}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="608135" y="34700309"/>
+          <a:ext cx="2505807" cy="1844552"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>586154</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>3640035</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62D75BCE-AFEE-B65D-020A-95938492EFE2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="608135" y="36788481"/>
+          <a:ext cx="3993173" cy="3640035"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -787,10 +1893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513C0935-569C-4726-AB72-325CD3527487}">
-  <dimension ref="A2:P24"/>
+  <dimension ref="A2:P70"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,7 +1914,7 @@
   <sheetData>
     <row r="2" spans="2:6" ht="24" x14ac:dyDescent="0.4">
       <c r="B2" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C2" s="6"/>
     </row>
@@ -818,7 +1924,7 @@
     </row>
     <row r="4" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C4" s="7"/>
     </row>
@@ -827,10 +1933,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -838,10 +1944,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -849,10 +1955,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>39</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -860,37 +1966,48 @@
         <v>4</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
@@ -898,10 +2015,10 @@
         <v>18</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -909,10 +2026,10 @@
         <v>18</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
@@ -920,10 +2037,10 @@
         <v>18</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
@@ -931,10 +2048,10 @@
         <v>18</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -942,10 +2059,10 @@
         <v>18</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -953,10 +2070,10 @@
         <v>18</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
@@ -964,50 +2081,353 @@
         <v>18</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D20" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="D21" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="7"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C24" s="7"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
         <v>1</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>46</v>
+      <c r="C25" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D27" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D28" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D29" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>3</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="167.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="1">
+        <v>2</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="163.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="1">
+        <v>3</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="318.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="1">
+        <v>4</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="1">
+        <v>1</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="109.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="1">
+        <v>2</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" ht="212.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="1">
+        <v>3</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" ht="204" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="1">
+        <v>4</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B50" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="1">
+        <v>0</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="1">
+        <v>1</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" ht="158.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="1">
+        <v>2</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" ht="105.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="1">
+        <v>3</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" ht="168.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="1">
+        <v>4</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" ht="132" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="1">
+        <v>5</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="1">
+        <v>6</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B63" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="1">
+        <v>1</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" ht="172.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="1">
+        <v>2</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" ht="149.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="1">
+        <v>3</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" ht="295.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="1">
+        <v>4</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2AB3B6-EFA3-48EC-8700-D49BE51BAD05}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,25 +2447,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>104</v>
+        <v>48</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -1076,41 +2496,6 @@
       </c>
       <c r="R1" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H2" t="s">
-        <v>70</v>
-      </c>
-      <c r="I2" t="s">
-        <v>71</v>
-      </c>
-      <c r="J2" t="s">
-        <v>72</v>
-      </c>
-      <c r="K2" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1120,10 +2505,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFEA08D4-B2B6-4A54-8AB6-F9ED1430102C}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,25 +2530,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>104</v>
+        <v>48</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -1194,35 +2579,6 @@
       </c>
       <c r="R1" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H2" t="s">
-        <v>78</v>
-      </c>
-      <c r="I2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J2" t="s">
-        <v>80</v>
-      </c>
-      <c r="K2" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1232,10 +2588,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B503794-0BF6-42D5-B048-A14E2079B383}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1257,25 +2613,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>104</v>
+        <v>48</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -1310,31 +2666,89 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2" t="s">
-        <v>87</v>
+        <v>24</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>195</v>
       </c>
       <c r="J2" t="s">
-        <v>88</v>
-      </c>
-      <c r="K2" t="s">
-        <v>89</v>
+        <v>196</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="J3" t="s">
+        <v>203</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="J4" t="s">
+        <v>210</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -1344,10 +2758,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42A6DF7B-9CA8-403F-9B14-EE84D961C3AB}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1371,25 +2785,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>104</v>
+        <v>48</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -1420,29 +2834,6 @@
       </c>
       <c r="R1" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G2" t="s">
-        <v>91</v>
-      </c>
-      <c r="J2" t="s">
-        <v>93</v>
-      </c>
-      <c r="K2" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1474,25 +2865,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>104</v>
+        <v>48</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -1532,10 +2923,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1F9A6CA-3282-4E5C-BCF2-C3D7AB9189BF}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V18" sqref="V18"/>
+      <selection activeCell="AC13" sqref="AC13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1553,25 +2944,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>104</v>
+        <v>48</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -1604,26 +2995,180 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="9" t="s">
         <v>51</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1633,10 +3178,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D47F3228-4157-4898-8BD9-96B689C5F379}">
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+      <selection activeCell="G2" sqref="G2:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1656,25 +3201,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>104</v>
+        <v>48</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -1705,6 +3250,226 @@
       </c>
       <c r="R1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1714,10 +3479,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB417B5A-E19E-494E-9B0E-D0062BC87F80}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1738,25 +3503,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>104</v>
+        <v>48</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -1787,29 +3552,6 @@
       </c>
       <c r="R1" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" t="s">
-        <v>53</v>
-      </c>
-      <c r="L2" t="s">
-        <v>54</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>100</v>
-      </c>
-      <c r="O2" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1819,10 +3561,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{626E7753-0163-4776-8D8A-1F41AD873694}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1844,25 +3586,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>104</v>
+        <v>48</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -1893,26 +3635,6 @@
       </c>
       <c r="R1" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" t="s">
-        <v>57</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>100</v>
-      </c>
-      <c r="R2" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1922,10 +3644,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B277CDE-02CF-4003-A084-D4F570CBCB08}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1944,25 +3666,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>104</v>
+        <v>48</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -1999,36 +3721,823 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" t="s">
-        <v>59</v>
+      <c r="B2" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>128</v>
       </c>
       <c r="L2" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>60</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="L3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>100</v>
+      </c>
+      <c r="O3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="L4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>100</v>
+      </c>
+      <c r="O4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="L5" t="s">
+        <v>43</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>100</v>
+      </c>
+      <c r="O5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="L6" t="s">
+        <v>43</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>100</v>
+      </c>
+      <c r="O6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="L7" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>100</v>
+      </c>
+      <c r="O7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="L8" t="s">
+        <v>43</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>100</v>
+      </c>
+      <c r="O8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="L9" t="s">
+        <v>43</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>100</v>
+      </c>
+      <c r="O9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="L10" t="s">
+        <v>43</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>100</v>
+      </c>
+      <c r="O10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="L11" t="s">
+        <v>43</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>100</v>
+      </c>
+      <c r="O11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="L12" t="s">
+        <v>43</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>100</v>
+      </c>
+      <c r="O12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="L13" t="s">
+        <v>43</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>100</v>
+      </c>
+      <c r="O13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="L14" t="s">
+        <v>43</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>100</v>
+      </c>
+      <c r="O14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="L15" t="s">
+        <v>43</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>100</v>
+      </c>
+      <c r="O15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="L16" t="s">
+        <v>43</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>100</v>
+      </c>
+      <c r="O16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="L17" t="s">
+        <v>43</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>100</v>
+      </c>
+      <c r="O17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="L18" t="s">
+        <v>43</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>100</v>
+      </c>
+      <c r="O18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="L19" t="s">
+        <v>43</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>100</v>
+      </c>
+      <c r="O19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="L20" t="s">
+        <v>43</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>100</v>
+      </c>
+      <c r="O20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="L21" t="s">
+        <v>43</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>100</v>
+      </c>
+      <c r="O21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="L22" t="s">
+        <v>43</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>100</v>
+      </c>
+      <c r="O22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="L23" t="s">
+        <v>43</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>100</v>
+      </c>
+      <c r="O23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="L24" t="s">
+        <v>43</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>100</v>
+      </c>
+      <c r="O24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="L25" t="s">
+        <v>43</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>100</v>
+      </c>
+      <c r="O25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="L26" t="s">
+        <v>43</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>100</v>
+      </c>
+      <c r="O26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="L27" t="s">
+        <v>43</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>100</v>
+      </c>
+      <c r="O27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="L28" t="s">
+        <v>43</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>100</v>
+      </c>
+      <c r="O28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="L29" t="s">
+        <v>43</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>100</v>
+      </c>
+      <c r="O29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="L30" t="s">
+        <v>43</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>100</v>
+      </c>
+      <c r="O30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="L31" t="s">
+        <v>43</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>100</v>
+      </c>
+      <c r="O31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="L32" t="s">
+        <v>43</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>100</v>
+      </c>
+      <c r="O32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="L33" t="s">
+        <v>43</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>100</v>
+      </c>
+      <c r="O33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="L34" t="s">
+        <v>43</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>100</v>
+      </c>
+      <c r="O34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="L35" t="s">
+        <v>43</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>100</v>
+      </c>
+      <c r="O35" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B16">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="SPARE">
+      <formula>NOT(ISERROR(SEARCH("SPARE",B16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="SPARE">
+      <formula>NOT(ISERROR(SEARCH("SPARE",B16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="SPARE">
+      <formula>NOT(ISERROR(SEARCH("SPARE",B16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="SPARE">
+      <formula>NOT(ISERROR(SEARCH("SPARE",B16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="SPARE">
+      <formula>NOT(ISERROR(SEARCH("SPARE",B30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="SPARE">
+      <formula>NOT(ISERROR(SEARCH("SPARE",B30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="SPARE">
+      <formula>NOT(ISERROR(SEARCH("SPARE",B30)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="SPARE">
+      <formula>NOT(ISERROR(SEARCH("SPARE",B30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAE71E9E-F5D3-45EF-8C68-1F53351AF2DE}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2050,25 +4559,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>104</v>
+        <v>48</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -2099,26 +4608,6 @@
       </c>
       <c r="R1" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" t="s">
-        <v>62</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>50</v>
-      </c>
-      <c r="R2" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2128,10 +4617,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{983E1042-8ABE-4A41-AAC4-DD53BAE52DC8}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2154,25 +4643,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>104</v>
+        <v>48</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -2203,50 +4692,6 @@
       </c>
       <c r="R1" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G2" t="s">
-        <v>99</v>
-      </c>
-      <c r="J2" t="s">
-        <v>98</v>
-      </c>
-      <c r="K2" t="s">
-        <v>100</v>
-      </c>
-      <c r="L2" t="s">
-        <v>107</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>5</v>
-      </c>
-      <c r="O2" t="s">
-        <v>60</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>100</v>
-      </c>
-      <c r="R2" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: fix bug when AI Type select
</commit_message>
<xml_diff>
--- a/EXCEL_MASTER.xlsx
+++ b/EXCEL_MASTER.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\2025\ScriptGenerator\Code\toDeploy\logic_designer_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC7C9A3B-8539-4580-A7BE-C270938BEA0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA20068-AC65-4E3E-92AB-1CF1785D280D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CA16010F-BA2C-49E5-B591-C71559C6A31C}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="262">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -125,9 +125,6 @@
     <t>SIO21</t>
   </si>
   <si>
-    <t>If you still do not have any reference to analog range and engineering unit, please DO NOT leave it empty (fill with e.g, 0, 100, and %)</t>
-  </si>
-  <si>
     <t>Digital Input (NPAS_DI_STS Only)</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>NPAS_PID**</t>
   </si>
   <si>
-    <t>Please enter your IO data into EVERY column on the relevant TYPE of the type sheet*</t>
-  </si>
-  <si>
     <t>Filling up the excel file:</t>
   </si>
   <si>
@@ -176,9 +170,6 @@
     <t>.</t>
   </si>
   <si>
-    <t>Fill the first column with "TYPE" (without " ") on every row that has IO Data</t>
-  </si>
-  <si>
     <t>I_Anlg</t>
   </si>
   <si>
@@ -197,9 +188,6 @@
     <t>TAG_OUT2</t>
   </si>
   <si>
-    <t>For analog input, please specify ANLG_IN_TYPE (I_Anlg or I_Temp)</t>
-  </si>
-  <si>
     <t>ESD-000</t>
   </si>
   <si>
@@ -689,12 +677,6 @@
     <t>:</t>
   </si>
   <si>
-    <t>DON'T REMOVE ANY SHEET OR MODIFY THE ORDER OF THE SHEETS. ONLY MODIFY CELLS/CONTENT OF THE SHEET</t>
-  </si>
-  <si>
-    <t>All of the output files will be generate at {.exe directory}/Output folder</t>
-  </si>
-  <si>
     <t>Those files are:</t>
   </si>
   <si>
@@ -791,14 +773,88 @@
     <t>Add the new POU into the Task. Do rearrange as needed since the conversion file is untidy</t>
   </si>
   <si>
-    <t>The pre-filled value is set as an example</t>
+    <t>Use the MASTER.csv file to debug when the program mention 'Line ## : invalid category'</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Please enter your IO data into EVERY column on the relevant TYPE of the type sheet*. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DO NOT FILL 'MASTER' SHEET</t>
+    </r>
+  </si>
+  <si>
+    <t>DON'T REMOVE ANY SHEET OR MODIFY THE ORDER OF THE SHEETS. ONLY MODIFY CELLS/CONTENT OF THE TYPE SHEET</t>
+  </si>
+  <si>
+    <t>If you still do not have any reference to analog range and engineering unit, please DO NOT leave it empty (fill with i.e, 0, 100, and %)</t>
+  </si>
+  <si>
+    <t>For analog input, please specify ANLG_IN_TYPE with: I_Anlg or I_Temp</t>
+  </si>
+  <si>
+    <t>Fill the first column with "TYPE" (without " ") on every row that has IO Data. The pre-filled value is set as an example, remove if not needed</t>
+  </si>
+  <si>
+    <t>If done correctly, all of the output files will be generate at {.exe directory}/Output folder.</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>If the Output folder is not generated, move the .exe and .xlsx file location in D:/ partition (or where the execution don't need admin previlleges)</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Permission error</t>
+  </si>
+  <si>
+    <t>Cause: You perhaps are re-executing LOGIC_GENERATOR and have the output file(s) open.</t>
+  </si>
+  <si>
+    <t>Solution: Close the file(s)  (MASTER.csv/LOC_VAR.xlsx/DEV_LABEL.csv/STRUCT_TEXT.txt).</t>
+  </si>
+  <si>
+    <t>Common Error/Warning</t>
+  </si>
+  <si>
+    <t>AI Type Wrong Definition at line {idx}. Must be either 'I_Anlg' or 'I_Temp'</t>
+  </si>
+  <si>
+    <t>Solution: Define data for column 'ANLG_IN_TYPE' with either 'I_Anlg' or 'I_Temp'</t>
+  </si>
+  <si>
+    <t>Cause: You define data for column 'ANLG_IN_TYPE' wrong. Check affected data at line {idx} on MASTER.csv</t>
+  </si>
+  <si>
+    <t>Cause: You define data for column 'CATEGORY' wrong. Check affected data at line {idx} on MASTER.csv</t>
+  </si>
+  <si>
+    <t>Solution: Define data for column 'CATEGORY' with: DI/DO/AI/AO/PVI/MLD/PID/SIO22/SIO12/SIO21/SIO11 only</t>
+  </si>
+  <si>
+    <t>Line {idx} invalid category. Check MASTER.csv</t>
+  </si>
+  <si>
+    <t>If im still here, please report your error to: faishal.tahsiin@yokogawa.com cc: ferdian.pradana@yokogawa.com with subject: LOGIC_GENERATOR_ERR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -832,6 +888,22 @@
       <i/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -884,7 +956,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -914,6 +986,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1006,13 +1083,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>65942</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>21982</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>2080846</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1049,13 +1126,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>157528</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>2036885</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1093,13 +1170,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>168520</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>4030491</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1137,13 +1214,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>300766</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>1370135</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1181,13 +1258,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>58616</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>2638693</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1225,13 +1302,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>481476</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>2535116</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1269,13 +1346,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>26748</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>1970943</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1313,13 +1390,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>1247602</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1357,13 +1434,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>234461</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>2066701</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1401,13 +1478,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>403513</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>1638529</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1445,13 +1522,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>600808</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>2111514</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1489,13 +1566,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>315057</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>1844553</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1533,13 +1610,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>586154</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>3640035</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1565,6 +1642,50 @@
         <a:xfrm>
           <a:off x="608135" y="36788481"/>
           <a:ext cx="3993173" cy="3640035"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>20910</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>838317</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9D4D645-BE3A-AA9B-81B4-18298876A494}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="608135" y="44613635"/>
+          <a:ext cx="2819794" cy="838317"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1893,527 +2014,636 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513C0935-569C-4726-AB72-325CD3527487}">
-  <dimension ref="A2:P70"/>
+  <dimension ref="A2:P84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="15" customWidth="1"/>
     <col min="2" max="2" width="4.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="1" style="8" customWidth="1"/>
     <col min="4" max="4" width="3.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="1" customWidth="1"/>
     <col min="6" max="14" width="9.140625" style="1"/>
     <col min="15" max="15" width="13.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="4.42578125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="17.5703125" style="1" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="24" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.4">
       <c r="B2" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C2" s="6"/>
     </row>
-    <row r="3" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="4"/>
       <c r="C3" s="6"/>
     </row>
-    <row r="4" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="15">
+        <v>1</v>
+      </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C4" s="7"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>2</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>3</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>4</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="1">
-        <v>0</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D12" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E12" s="1" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D15" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D16" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D17" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D18" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D20" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D20" s="12" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="15">
+        <v>2</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="1">
+        <v>2</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D26" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D21" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="C24" s="7"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="1">
-        <v>1</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="1">
-        <v>2</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E26" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D27" s="14" t="s">
         <v>18</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D28" s="14" t="s">
         <v>18</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B29" s="1">
+        <v>3</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D31" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="15">
+        <v>3</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="167.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B36" s="1">
+        <v>2</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D29" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="1">
+    <row r="37" spans="1:4" ht="163.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B38" s="1">
         <v>3</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B32" s="3" t="s">
+      <c r="C38" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="318.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B40" s="1">
+        <v>4</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="15">
+        <v>4</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B43" s="1">
+        <v>1</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="109.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B45" s="1">
+        <v>2</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="212.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B47" s="1">
+        <v>3</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="204" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B49" s="1">
+        <v>4</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="15">
+        <v>5</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B52" s="1">
+        <v>0</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B53" s="1">
+        <v>1</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1">
+    <row r="54" spans="1:4" ht="158.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B55" s="1">
+        <v>2</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="105.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B57" s="1">
+        <v>3</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="168.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B59" s="1">
+        <v>4</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="132" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B61" s="1">
+        <v>5</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B62" s="1">
+        <v>6</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="15">
+        <v>6</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B65" s="1">
         <v>1</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" ht="167.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="1">
+      <c r="C65" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="172.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B67" s="1">
         <v>2</v>
       </c>
-      <c r="C35" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" ht="163.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="1">
+      <c r="C67" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="149.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B69" s="1">
         <v>3</v>
       </c>
-      <c r="C37" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" ht="318.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="1">
+      <c r="C69" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="295.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B71" s="1">
         <v>4</v>
       </c>
-      <c r="C39" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="1">
-        <v>1</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" ht="109.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="1">
-        <v>2</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" ht="212.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="1">
-        <v>3</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" ht="204" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="1">
-        <v>4</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B50" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="1">
-        <v>0</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="1">
-        <v>1</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" ht="158.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="1">
-        <v>2</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" ht="105.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="1">
-        <v>3</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" ht="168.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="1">
-        <v>4</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" ht="132" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B60" s="1">
-        <v>5</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D60" s="1" t="s">
+      <c r="C71" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="1">
-        <v>6</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="63" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B63" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B64" s="1">
-        <v>1</v>
-      </c>
-      <c r="C64" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="65" spans="2:4" ht="172.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="1">
-        <v>2</v>
-      </c>
-      <c r="C66" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="67" spans="2:4" ht="149.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="1">
-        <v>3</v>
-      </c>
-      <c r="C68" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="69" spans="2:4" ht="295.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="1">
-        <v>4</v>
-      </c>
-      <c r="C70" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>246</v>
+    <row r="72" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A72" s="2"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="15">
+        <v>7</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B74" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D74" s="17" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="69.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D76" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D77" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B78" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D78" s="17" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D79" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D80" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B81" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D81" s="17" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D82" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D83" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B84" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -2447,25 +2677,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -2530,25 +2760,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -2613,25 +2843,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -2669,28 +2899,28 @@
         <v>24</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="G2" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="J2" t="s">
         <v>192</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="K2" s="10" t="s">
         <v>191</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="J2" t="s">
-        <v>196</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -2698,28 +2928,28 @@
         <v>24</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="G3" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="J3" t="s">
         <v>199</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="K3" s="10" t="s">
         <v>198</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="J3" t="s">
-        <v>203</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -2727,28 +2957,28 @@
         <v>24</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="G4" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="J4" t="s">
         <v>206</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="K4" s="10" t="s">
         <v>205</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="J4" t="s">
-        <v>210</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -2785,25 +3015,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -2846,7 +3076,7 @@
   <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2865,25 +3095,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -2944,25 +3174,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -3000,10 +3230,10 @@
         <v>19</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3011,10 +3241,10 @@
         <v>19</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3022,10 +3252,10 @@
         <v>19</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3033,10 +3263,10 @@
         <v>19</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3044,10 +3274,10 @@
         <v>19</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3055,10 +3285,10 @@
         <v>19</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3066,10 +3296,10 @@
         <v>19</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3077,10 +3307,10 @@
         <v>19</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3088,10 +3318,10 @@
         <v>19</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3099,10 +3329,10 @@
         <v>19</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3110,10 +3340,10 @@
         <v>19</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3121,10 +3351,10 @@
         <v>19</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3132,10 +3362,10 @@
         <v>19</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3143,10 +3373,10 @@
         <v>19</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3154,10 +3384,10 @@
         <v>19</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -3165,10 +3395,10 @@
         <v>19</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -3201,25 +3431,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -3257,10 +3487,10 @@
         <v>9</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3268,10 +3498,10 @@
         <v>9</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3279,10 +3509,10 @@
         <v>9</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3290,10 +3520,10 @@
         <v>9</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3301,10 +3531,10 @@
         <v>9</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3312,10 +3542,10 @@
         <v>9</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3323,10 +3553,10 @@
         <v>9</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3334,10 +3564,10 @@
         <v>9</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3345,10 +3575,10 @@
         <v>9</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3356,10 +3586,10 @@
         <v>9</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3367,10 +3597,10 @@
         <v>9</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3378,10 +3608,10 @@
         <v>9</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3389,10 +3619,10 @@
         <v>9</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3400,10 +3630,10 @@
         <v>9</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
@@ -3411,10 +3641,10 @@
         <v>9</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -3422,10 +3652,10 @@
         <v>9</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -3433,10 +3663,10 @@
         <v>9</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -3444,10 +3674,10 @@
         <v>9</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -3455,10 +3685,10 @@
         <v>9</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -3466,10 +3696,10 @@
         <v>9</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -3503,25 +3733,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -3586,25 +3816,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -3666,25 +3896,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -3722,13 +3952,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="L2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -3737,7 +3967,7 @@
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -3745,13 +3975,13 @@
         <v>7</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="L3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -3760,7 +3990,7 @@
         <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -3768,13 +3998,13 @@
         <v>7</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="L4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -3783,7 +4013,7 @@
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -3791,13 +4021,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="L5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -3806,7 +4036,7 @@
         <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -3814,13 +4044,13 @@
         <v>7</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="L6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -3829,7 +4059,7 @@
         <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -3837,13 +4067,13 @@
         <v>7</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="L7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -3852,7 +4082,7 @@
         <v>100</v>
       </c>
       <c r="O7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -3860,13 +4090,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="L8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -3875,7 +4105,7 @@
         <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -3883,13 +4113,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="L9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -3898,7 +4128,7 @@
         <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -3906,13 +4136,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="L10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -3921,7 +4151,7 @@
         <v>100</v>
       </c>
       <c r="O10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -3929,13 +4159,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="L11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -3944,7 +4174,7 @@
         <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -3952,13 +4182,13 @@
         <v>7</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="L12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -3967,7 +4197,7 @@
         <v>100</v>
       </c>
       <c r="O12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -3975,13 +4205,13 @@
         <v>7</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="L13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -3990,7 +4220,7 @@
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -3998,13 +4228,13 @@
         <v>7</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="L14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -4013,7 +4243,7 @@
         <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -4021,13 +4251,13 @@
         <v>7</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="L15" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -4036,7 +4266,7 @@
         <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -4044,13 +4274,13 @@
         <v>7</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="L16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M16">
         <v>0</v>
@@ -4059,7 +4289,7 @@
         <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -4067,13 +4297,13 @@
         <v>7</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="L17" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M17">
         <v>0</v>
@@ -4082,7 +4312,7 @@
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -4090,13 +4320,13 @@
         <v>7</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="L18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M18">
         <v>0</v>
@@ -4105,7 +4335,7 @@
         <v>100</v>
       </c>
       <c r="O18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -4113,13 +4343,13 @@
         <v>7</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="L19" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M19">
         <v>0</v>
@@ -4128,7 +4358,7 @@
         <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -4136,13 +4366,13 @@
         <v>7</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="L20" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M20">
         <v>0</v>
@@ -4151,7 +4381,7 @@
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -4159,13 +4389,13 @@
         <v>7</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="L21" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M21">
         <v>0</v>
@@ -4174,7 +4404,7 @@
         <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -4182,13 +4412,13 @@
         <v>7</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="L22" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M22">
         <v>0</v>
@@ -4197,7 +4427,7 @@
         <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -4205,13 +4435,13 @@
         <v>7</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="L23" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M23">
         <v>0</v>
@@ -4220,7 +4450,7 @@
         <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -4228,13 +4458,13 @@
         <v>7</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="L24" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M24">
         <v>0</v>
@@ -4243,7 +4473,7 @@
         <v>100</v>
       </c>
       <c r="O24" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -4251,13 +4481,13 @@
         <v>7</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="L25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M25">
         <v>0</v>
@@ -4266,7 +4496,7 @@
         <v>100</v>
       </c>
       <c r="O25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -4274,13 +4504,13 @@
         <v>7</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="L26" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M26">
         <v>0</v>
@@ -4289,7 +4519,7 @@
         <v>100</v>
       </c>
       <c r="O26" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -4297,13 +4527,13 @@
         <v>7</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="L27" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M27">
         <v>0</v>
@@ -4312,7 +4542,7 @@
         <v>100</v>
       </c>
       <c r="O27" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -4320,13 +4550,13 @@
         <v>7</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="L28" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M28">
         <v>0</v>
@@ -4335,7 +4565,7 @@
         <v>100</v>
       </c>
       <c r="O28" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -4343,13 +4573,13 @@
         <v>7</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="L29" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M29">
         <v>0</v>
@@ -4358,7 +4588,7 @@
         <v>100</v>
       </c>
       <c r="O29" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -4366,13 +4596,13 @@
         <v>7</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="L30" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M30">
         <v>0</v>
@@ -4381,7 +4611,7 @@
         <v>100</v>
       </c>
       <c r="O30" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -4389,13 +4619,13 @@
         <v>7</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="L31" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M31">
         <v>0</v>
@@ -4404,7 +4634,7 @@
         <v>100</v>
       </c>
       <c r="O31" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -4412,13 +4642,13 @@
         <v>7</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="L32" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M32">
         <v>0</v>
@@ -4427,7 +4657,7 @@
         <v>100</v>
       </c>
       <c r="O32" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -4435,13 +4665,13 @@
         <v>7</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="L33" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M33">
         <v>0</v>
@@ -4450,7 +4680,7 @@
         <v>100</v>
       </c>
       <c r="O33" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
@@ -4458,13 +4688,13 @@
         <v>7</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="L34" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M34">
         <v>0</v>
@@ -4473,7 +4703,7 @@
         <v>100</v>
       </c>
       <c r="O34" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
@@ -4481,13 +4711,13 @@
         <v>7</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="L35" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M35">
         <v>0</v>
@@ -4496,7 +4726,7 @@
         <v>100</v>
       </c>
       <c r="O35" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -4559,25 +4789,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -4643,25 +4873,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
mod: reroute handler to handler folder
</commit_message>
<xml_diff>
--- a/EXCEL_MASTER.xlsx
+++ b/EXCEL_MASTER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\2025\ScriptGenerator\Code\toDeploy\logic_designer_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA20068-AC65-4E3E-92AB-1CF1785D280D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0402E23C-9933-427E-B58A-A3BB0C4958CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CA16010F-BA2C-49E5-B591-C71559C6A31C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{CA16010F-BA2C-49E5-B591-C71559C6A31C}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="9" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="264">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -847,7 +847,13 @@
     <t>Line {idx} invalid category. Check MASTER.csv</t>
   </si>
   <si>
-    <t>If im still here, please report your error to: faishal.tahsiin@yokogawa.com cc: ferdian.pradana@yokogawa.com with subject: LOGIC_GENERATOR_ERR</t>
+    <t>Report your error to: faishal.tahsiin@yokogawa.com cc: ferdian.pradana@yokogawa.com with subject: LOGIC_GENERATOR_ERR</t>
+  </si>
+  <si>
+    <t>I'll reply if I'm still here</t>
+  </si>
+  <si>
+    <t>I_Anlgz</t>
   </si>
 </sst>
 </file>
@@ -2014,10 +2020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513C0935-569C-4726-AB72-325CD3527487}">
-  <dimension ref="A2:P84"/>
+  <dimension ref="A2:P85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2644,6 +2650,11 @@
       </c>
       <c r="D84" s="1" t="s">
         <v>261</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D85" s="1" t="s">
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -3876,8 +3887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B277CDE-02CF-4003-A084-D4F570CBCB08}">
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3958,7 +3969,7 @@
         <v>124</v>
       </c>
       <c r="L2" t="s">
-        <v>40</v>
+        <v>263</v>
       </c>
       <c r="M2">
         <v>0</v>

</xml_diff>

<commit_message>
add: add distribution packaged .exe file in /dist
</commit_message>
<xml_diff>
--- a/EXCEL_MASTER.xlsx
+++ b/EXCEL_MASTER.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\2025\ScriptGenerator\Code\toDeploy\logic_designer_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0402E23C-9933-427E-B58A-A3BB0C4958CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A412A351-AE5E-47AC-A657-877856CBD0DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{CA16010F-BA2C-49E5-B591-C71559C6A31C}"/>
   </bookViews>
@@ -3888,7 +3888,7 @@
   <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>